<commit_message>
balancing and making helper cards
About to do my first playtest
</commit_message>
<xml_diff>
--- a/game.xlsx
+++ b/game.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="65">
   <si>
     <t>Name</t>
   </si>
@@ -216,26 +216,29 @@
     <t>8 HP. 2 ATK.</t>
   </si>
   <si>
-    <t>4 HP. 3 ATK.</t>
-  </si>
-  <si>
     <t>3 HP. 3 ATK.
 Insta-slaughter: Whacking Plank</t>
   </si>
   <si>
-    <t>3 HP. 2 ATK. 
+    <t>4:1:1:1 Metal:Fabric:Oil:Duct Tape</t>
+  </si>
+  <si>
+    <t>Max</t>
+  </si>
+  <si>
+    <t>6 HP. 2 ATK. 
 Insta-slaughter: Tote Bag</t>
   </si>
   <si>
-    <t>4:1:1:1 Metal:Fabric:Oil:Duct Tape</t>
-  </si>
-  <si>
-    <t>6 HP. 2 ATK.
+    <t>7 HP. 2 ATK.</t>
+  </si>
+  <si>
+    <t>12 HP. 2 ATK.
 Insta-slaughter: Bandages</t>
   </si>
   <si>
-    <t>2 HP. 2 ATK.
-Insta-slaughter: Fireball</t>
+    <t>5 HP. 3 ATK.
+Insta-slaughter: Strong magnet</t>
   </si>
 </sst>
 </file>
@@ -279,7 +282,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -301,6 +304,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -616,7 +622,7 @@
   <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -685,13 +691,13 @@
         <v>32</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="I2" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>21</v>
       </c>
@@ -714,7 +720,7 @@
         <v>25</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I3" s="3">
         <v>2</v>
@@ -772,7 +778,7 @@
         <v>43</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="I5" s="3">
         <v>4</v>
@@ -800,14 +806,14 @@
       <c r="G6" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="H6" s="7" t="s">
         <v>10</v>
       </c>
       <c r="I6" s="3">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>14</v>
       </c>
@@ -829,8 +835,8 @@
       <c r="G7" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="H7" s="2" t="s">
-        <v>58</v>
+      <c r="H7" s="7" t="s">
+        <v>64</v>
       </c>
       <c r="I7" s="3">
         <v>6</v>
@@ -882,13 +888,13 @@
         <v>5</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>43</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I9" s="3">
         <v>1</v>
@@ -1031,198 +1037,226 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:F9"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="9.140625" style="1"/>
-    <col min="5" max="5" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="57.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="1"/>
+    <col min="2" max="2" width="4.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="9.140625" style="1"/>
+    <col min="6" max="6" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="57.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B2" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2" s="1">
+        <v>0</v>
+      </c>
+      <c r="D2" s="1">
         <v>2</v>
       </c>
-      <c r="D2" s="1">
-        <v>0</v>
-      </c>
       <c r="E2" s="1">
-        <v>1</v>
-      </c>
-      <c r="F2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="1">
+        <v>1</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B3" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C3" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D3" s="1">
         <v>1</v>
       </c>
       <c r="E3" s="1">
-        <v>0</v>
-      </c>
-      <c r="F3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>51</v>
       </c>
       <c r="B4" s="1">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1">
         <v>3</v>
       </c>
-      <c r="C4" s="1">
-        <v>0</v>
-      </c>
       <c r="D4" s="1">
         <v>0</v>
       </c>
       <c r="E4" s="1">
-        <v>1</v>
-      </c>
-      <c r="F4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F4" s="1">
+        <v>1</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B5" s="1">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1">
         <v>3</v>
       </c>
-      <c r="C5" s="1">
-        <v>0</v>
-      </c>
       <c r="D5" s="1">
         <v>0</v>
       </c>
       <c r="E5" s="1">
         <v>0</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" s="1">
+        <v>0</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>43</v>
       </c>
       <c r="B6" s="1">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1">
         <v>2</v>
       </c>
-      <c r="C6" s="1">
-        <v>0</v>
-      </c>
       <c r="D6" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E6" s="1">
-        <v>0</v>
-      </c>
-      <c r="F6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B7" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C7" s="1">
+        <v>0</v>
+      </c>
+      <c r="D7" s="1">
         <v>2</v>
       </c>
-      <c r="D7" s="1">
-        <v>0</v>
-      </c>
       <c r="E7" s="1">
-        <v>1</v>
-      </c>
-      <c r="F7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F7" s="1">
+        <v>1</v>
+      </c>
+      <c r="G7" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>49</v>
       </c>
       <c r="B8" s="1">
+        <v>1</v>
+      </c>
+      <c r="C8" s="1">
         <v>2</v>
       </c>
-      <c r="C8" s="1">
-        <v>0</v>
-      </c>
       <c r="D8" s="1">
         <v>0</v>
       </c>
       <c r="E8" s="1">
         <v>0</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F8" s="1">
+        <v>0</v>
+      </c>
+      <c r="G8" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>45</v>
       </c>
       <c r="B9" s="1">
+        <v>1</v>
+      </c>
+      <c r="C9" s="1">
         <v>12</v>
       </c>
-      <c r="C9" s="1">
+      <c r="D9" s="1">
         <v>8</v>
       </c>
-      <c r="D9" s="1">
+      <c r="E9" s="1">
         <v>6</v>
       </c>
-      <c r="E9" s="1">
+      <c r="F9" s="1">
         <v>4</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="G9" s="1" t="s">
         <v>44</v>
       </c>
     </row>
@@ -1248,12 +1282,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
     </row>
     <row r="2" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="4" t="s">

</xml_diff>

<commit_message>
some cleanup and other ideas immediately after playtest
Ok NOW I'm gonna go to bed...
</commit_message>
<xml_diff>
--- a/game.xlsx
+++ b/game.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="74">
   <si>
     <t>Name</t>
   </si>
@@ -88,16 +88,10 @@
     <t>Curtain Ghost</t>
   </si>
   <si>
-    <t>1:1 for Metal:Fabric</t>
-  </si>
-  <si>
     <t>Big</t>
   </si>
   <si>
     <t>Major Ductwork</t>
-  </si>
-  <si>
-    <t>3 HP. 3 ATK. Insta-slaughter: Fireball</t>
   </si>
   <si>
     <t>Sprocket Bats</t>
@@ -213,32 +207,73 @@
     <t>Sewing Machine</t>
   </si>
   <si>
-    <t>8 HP. 2 ATK.</t>
+    <t>4:1:1:1 Metal:Fabric:Oil:Duct Tape</t>
+  </si>
+  <si>
+    <t>Max</t>
+  </si>
+  <si>
+    <t>7 HP. 2 ATK.</t>
+  </si>
+  <si>
+    <t>1:2 for Metal:Fabric</t>
+  </si>
+  <si>
+    <t>13 HP. 3 ATK. 
+Insta-slaughter: Fireball</t>
+  </si>
+  <si>
+    <t>Strong Magnet
+for 4 Metal</t>
+  </si>
+  <si>
+    <t>Fireball
+for 1 Fabric + 1 Oil</t>
+  </si>
+  <si>
+    <t>Bandages
+for 1 Fabric + 1 Duct Tape</t>
+  </si>
+  <si>
+    <t>12 HP. 2 ATK.
+Insta-slaughter: Use Bandages</t>
+  </si>
+  <si>
+    <t>5 HP. 3 ATK.
+Insta-slaughter: Use Strong Magnet</t>
   </si>
   <si>
     <t>3 HP. 3 ATK.
-Insta-slaughter: Whacking Plank</t>
-  </si>
-  <si>
-    <t>4:1:1:1 Metal:Fabric:Oil:Duct Tape</t>
-  </si>
-  <si>
-    <t>Max</t>
+Insta-slaughter: Have Whacking Plank</t>
+  </si>
+  <si>
+    <t>18 HP. 2 ATK.</t>
+  </si>
+  <si>
+    <t>Tote Bag
+for 3 Fabric</t>
+  </si>
+  <si>
+    <t>Whacking Plank
+for 3 Metal and 1 Duct tape</t>
+  </si>
+  <si>
+    <t>Strange Device
+for 3 Metal + 1 Duct Tape</t>
+  </si>
+  <si>
+    <t>Tape Dispensor
+for 2 Metal + 1 Oil</t>
+  </si>
+  <si>
+    <t>1:1 Oil:Duct tape</t>
+  </si>
+  <si>
+    <t>4 Metal for +1 ATK</t>
   </si>
   <si>
     <t>6 HP. 2 ATK. 
-Insta-slaughter: Tote Bag</t>
-  </si>
-  <si>
-    <t>7 HP. 2 ATK.</t>
-  </si>
-  <si>
-    <t>12 HP. 2 ATK.
-Insta-slaughter: Bandages</t>
-  </si>
-  <si>
-    <t>5 HP. 3 ATK.
-Insta-slaughter: Strong magnet</t>
+Insta-slaughter: Use Tote Bag</t>
   </si>
 </sst>
 </file>
@@ -622,7 +657,7 @@
   <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -633,8 +668,8 @@
     <col min="4" max="4" width="6.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="3.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="50.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="34.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.28515625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="35.42578125" style="2" customWidth="1"/>
     <col min="9" max="9" width="5" style="3" bestFit="1" customWidth="1"/>
     <col min="10" max="16384" width="9.140625" style="2"/>
   </cols>
@@ -659,13 +694,13 @@
         <v>5</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="H1" s="6" t="s">
         <v>6</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -685,21 +720,21 @@
         <v>1</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>32</v>
+        <v>60</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="I2" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>8</v>
@@ -714,13 +749,13 @@
         <v>3</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>25</v>
+        <v>61</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="I3" s="3">
         <v>2</v>
@@ -728,7 +763,7 @@
     </row>
     <row r="4" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>8</v>
@@ -743,10 +778,10 @@
         <v>1</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>35</v>
+        <v>62</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>10</v>
@@ -774,8 +809,8 @@
       <c r="F5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="2" t="s">
-        <v>43</v>
+      <c r="G5" s="7" t="s">
+        <v>70</v>
       </c>
       <c r="H5" s="7" t="s">
         <v>63</v>
@@ -784,7 +819,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>13</v>
       </c>
@@ -801,10 +836,10 @@
         <v>2</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>51</v>
+        <v>38</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>69</v>
       </c>
       <c r="H6" s="7" t="s">
         <v>10</v>
@@ -830,10 +865,10 @@
         <v>0</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>49</v>
+        <v>31</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>68</v>
       </c>
       <c r="H7" s="7" t="s">
         <v>64</v>
@@ -842,7 +877,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>15</v>
       </c>
@@ -859,24 +894,24 @@
         <v>0</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>16</v>
+        <v>58</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>36</v>
+        <v>67</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="I8" s="3">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C9" s="3">
         <v>5</v>
@@ -888,24 +923,24 @@
         <v>5</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="I9" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C10" s="3">
         <v>5</v>
@@ -916,8 +951,14 @@
       <c r="E10" s="3">
         <v>5</v>
       </c>
-      <c r="H10" s="2" t="s">
-        <v>19</v>
+      <c r="F10" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>59</v>
       </c>
       <c r="I10" s="3">
         <v>2</v>
@@ -925,10 +966,10 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C11" s="3">
         <v>5</v>
@@ -938,6 +979,9 @@
       </c>
       <c r="E11" s="3">
         <v>5</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>72</v>
       </c>
       <c r="I11" s="3">
         <v>3</v>
@@ -945,10 +989,10 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C12" s="3">
         <v>5</v>
@@ -960,7 +1004,7 @@
         <v>5</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I12" s="3">
         <v>4</v>
@@ -968,10 +1012,10 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C13" s="3">
         <v>5</v>
@@ -988,10 +1032,10 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C14" s="3">
         <v>5</v>
@@ -1003,7 +1047,7 @@
         <v>5</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I14" s="3">
         <v>6</v>
@@ -1011,10 +1055,10 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C15" s="3">
         <v>5</v>
@@ -1040,7 +1084,7 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1055,10 +1099,10 @@
   <sheetData>
     <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>2</v>
@@ -1070,15 +1114,15 @@
         <v>4</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
@@ -1096,12 +1140,12 @@
         <v>1</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B3" s="1">
         <v>2</v>
@@ -1119,12 +1163,12 @@
         <v>0</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B4" s="1">
         <v>1</v>
@@ -1142,12 +1186,12 @@
         <v>1</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B5" s="1">
         <v>1</v>
@@ -1165,12 +1209,12 @@
         <v>0</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B6" s="1">
         <v>1</v>
@@ -1188,12 +1232,12 @@
         <v>0</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B7" s="1">
         <v>2</v>
@@ -1211,12 +1255,12 @@
         <v>1</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B8" s="1">
         <v>1</v>
@@ -1234,12 +1278,12 @@
         <v>0</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B9" s="1">
         <v>1</v>
@@ -1257,7 +1301,7 @@
         <v>4</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1283,7 +1327,7 @@
   <sheetData>
     <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B1" s="9" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C1" s="9"/>
       <c r="D1" s="9"/>
@@ -1300,7 +1344,7 @@
         <v>4</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1326,7 +1370,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B4" s="1">
         <f>SUM(Cards!C9:C15)</f>
@@ -1347,7 +1391,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B5" s="1">
         <f>SUM(Cards!C2:C15)</f>

</xml_diff>

<commit_message>
more combat sim results, game content
Game content choices:
  * Sketched out the Big creatures stats
  * Some icons for Insta-slaughter
  * Made a "value" metric for each creature composition
  * Just hashed out the economy more overall
</commit_message>
<xml_diff>
--- a/game.xlsx
+++ b/game.xlsx
@@ -8,7 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Cards" sheetId="1" r:id="rId1"/>
-    <sheet name="Recipes" sheetId="2" r:id="rId2"/>
+    <sheet name="Tools" sheetId="2" r:id="rId2"/>
     <sheet name="Economy" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="86">
   <si>
     <t>Name</t>
   </si>
@@ -127,13 +127,7 @@
     <t>Bonus</t>
   </si>
   <si>
-    <t>Use once in battle for -5 Creature HP</t>
-  </si>
-  <si>
     <t>Strong Magnet</t>
-  </si>
-  <si>
-    <t>1 Oil for +1 ATK</t>
   </si>
   <si>
     <t>1 Oil for 2HP
@@ -153,9 +147,6 @@
     <t>The Crusher</t>
   </si>
   <si>
-    <t>Disassemble 1 Tool to raw materials, except duct tape.</t>
-  </si>
-  <si>
     <t>4:3:2:1 for Metal:Fabric:Oil:Duct Tape</t>
   </si>
   <si>
@@ -177,12 +168,6 @@
     <t>May convert 3/2/1 Metal/Fabric/Oil to 1 Duct Tape each Round</t>
   </si>
   <si>
-    <t>Use once for +1 Carry</t>
-  </si>
-  <si>
-    <t>Gain 2 HP after each battle</t>
-  </si>
-  <si>
     <t>Whacking Plank</t>
   </si>
   <si>
@@ -217,63 +202,121 @@
   </si>
   <si>
     <t>1:2 for Metal:Fabric</t>
-  </si>
-  <si>
-    <t>13 HP. 3 ATK. 
-Insta-slaughter: Fireball</t>
   </si>
   <si>
     <t>Strong Magnet
 for 4 Metal</t>
   </si>
   <si>
-    <t>Fireball
-for 1 Fabric + 1 Oil</t>
-  </si>
-  <si>
-    <t>Bandages
-for 1 Fabric + 1 Duct Tape</t>
-  </si>
-  <si>
-    <t>12 HP. 2 ATK.
-Insta-slaughter: Use Bandages</t>
-  </si>
-  <si>
-    <t>5 HP. 3 ATK.
-Insta-slaughter: Use Strong Magnet</t>
-  </si>
-  <si>
-    <t>3 HP. 3 ATK.
-Insta-slaughter: Have Whacking Plank</t>
-  </si>
-  <si>
-    <t>18 HP. 2 ATK.</t>
-  </si>
-  <si>
     <t>Tote Bag
 for 3 Fabric</t>
   </si>
   <si>
+    <t>Gain 3 HP after each battle</t>
+  </si>
+  <si>
+    <t>1:1 Oil:Duct Tape</t>
+  </si>
+  <si>
+    <t>13 HP. 3 ATK. 
+ ⃠ Use Fireball</t>
+  </si>
+  <si>
+    <t>Use in battle for -6 Creature HP</t>
+  </si>
+  <si>
+    <t>Use for +1 Carry</t>
+  </si>
+  <si>
+    <t>15 HP. 2 ATK.</t>
+  </si>
+  <si>
+    <t>8 HP. 3 ATK.
+ ⃠ Have Strong Magnet</t>
+  </si>
+  <si>
+    <t>12 HP. 2 ATK. 
+ ⃠ Use Tote Bag</t>
+  </si>
+  <si>
+    <t>14 HP. 2 ATK.
+ ⃠ Use Bandages</t>
+  </si>
+  <si>
+    <t>+1 ATK for 1 Oil</t>
+  </si>
+  <si>
+    <t>Strong Magnet
+for 3 Metal</t>
+  </si>
+  <si>
+    <t>1/2 Tote Bags
+for 2/4 Fabric</t>
+  </si>
+  <si>
+    <t>1:2 Metal:Fabric</t>
+  </si>
+  <si>
+    <t>20 HP. 4 ATK.</t>
+  </si>
+  <si>
+    <t>Est. Value</t>
+  </si>
+  <si>
+    <t>10 HP. 3 ATK.</t>
+  </si>
+  <si>
+    <t>16 HP. 3 ATK.
+ ⃠ Have Strong Magnet</t>
+  </si>
+  <si>
+    <t>+1 ATK for 4 Metal</t>
+  </si>
+  <si>
+    <t>3 HP. 3 ATK.
+ ⃠ Use Tote Bag</t>
+  </si>
+  <si>
+    <t>12 HP. 4 ATK
+⃠ Have Whacking Plank</t>
+  </si>
+  <si>
+    <t>17 HP. 4 ATK. 
+⃠ Have Strange Device</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+2 Duct Tape for Disassembling 1 Tool </t>
+  </si>
+  <si>
+    <t>+2 Metal and +2 Fabric for 2 Oil</t>
+  </si>
+  <si>
+    <t>Strange Device
+for 2 Metal, 1 Duct Tape</t>
+  </si>
+  <si>
     <t>Whacking Plank
-for 3 Metal and 1 Duct tape</t>
+for 3 Metal, 1 Duct tape</t>
+  </si>
+  <si>
+    <t>Bandages
+for 1 Fabric, 1 Duct Tape</t>
+  </si>
+  <si>
+    <t>Fireball
+for 1 Fabric, 1 Oil</t>
+  </si>
+  <si>
+    <t>Tape Dispensor
+for 2 Metal, 1 Oil</t>
   </si>
   <si>
     <t>Strange Device
-for 3 Metal + 1 Duct Tape</t>
+for 3 Metal, 1 Duct Tape</t>
   </si>
   <si>
     <t>Tape Dispensor
-for 2 Metal + 1 Oil</t>
-  </si>
-  <si>
-    <t>1:1 Oil:Duct tape</t>
-  </si>
-  <si>
-    <t>4 Metal for +1 ATK</t>
-  </si>
-  <si>
-    <t>6 HP. 2 ATK. 
-Insta-slaughter: Use Tote Bag</t>
+for 3 Metal, 1 Oil</t>
   </si>
 </sst>
 </file>
@@ -317,7 +360,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -345,6 +388,15 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -654,10 +706,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -667,14 +719,15 @@
     <col min="3" max="3" width="6.140625" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="3.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="50.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="34.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="25.28515625" style="2" customWidth="1"/>
     <col min="8" max="8" width="35.42578125" style="2" customWidth="1"/>
     <col min="9" max="9" width="5" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="2"/>
+    <col min="10" max="10" width="9.140625" style="12"/>
+    <col min="11" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -702,8 +755,11 @@
       <c r="I1" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="J1" s="11" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -723,16 +779,20 @@
         <v>25</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="I2" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="J2" s="12">
+        <f>C2/4 + D2/3+E2/2</f>
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>19</v>
       </c>
@@ -752,16 +812,20 @@
         <v>26</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>61</v>
+        <v>82</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="I3" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="J3" s="12">
+        <f t="shared" ref="J3:J15" si="0">C3/4 + D3/3+E3/2</f>
+        <v>1.8333333333333333</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>27</v>
       </c>
@@ -778,10 +842,10 @@
         <v>1</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>62</v>
+        <v>81</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>10</v>
@@ -789,8 +853,12 @@
       <c r="I4" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="J4" s="12">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
@@ -810,16 +878,20 @@
         <v>12</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>70</v>
+        <v>85</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="I5" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="J5" s="12">
+        <f t="shared" si="0"/>
+        <v>1.5833333333333333</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>13</v>
       </c>
@@ -836,19 +908,23 @@
         <v>2</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>69</v>
+        <v>84</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>10</v>
+        <v>71</v>
       </c>
       <c r="I6" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="J6" s="12">
+        <f t="shared" si="0"/>
+        <v>3.333333333333333</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>14</v>
       </c>
@@ -864,20 +940,24 @@
       <c r="E7" s="3">
         <v>0</v>
       </c>
-      <c r="F7" s="2" t="s">
-        <v>31</v>
+      <c r="F7" s="10" t="s">
+        <v>65</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>68</v>
+        <v>80</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I7" s="3">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="J7" s="12">
+        <f t="shared" si="0"/>
+        <v>1.9166666666666665</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>15</v>
       </c>
@@ -894,19 +974,23 @@
         <v>0</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="I8" s="3">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="J8" s="12">
+        <f t="shared" si="0"/>
+        <v>2.5833333333333335</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>18</v>
       </c>
@@ -923,19 +1007,23 @@
         <v>5</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>41</v>
+        <v>50</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>83</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="I9" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="J9" s="12">
+        <f t="shared" si="0"/>
+        <v>5.416666666666667</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
@@ -943,51 +1031,65 @@
         <v>16</v>
       </c>
       <c r="C10" s="3">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D10" s="3">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E10" s="3">
         <v>5</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>61</v>
+        <v>82</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I10" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J10" s="12">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C11" s="3">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D11" s="3">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E11" s="3">
-        <v>5</v>
-      </c>
-      <c r="F11" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H11" s="7" t="s">
         <v>72</v>
       </c>
       <c r="I11" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J11" s="12">
+        <f t="shared" si="0"/>
+        <v>2.5833333333333335</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>17</v>
       </c>
@@ -995,67 +1097,100 @@
         <v>16</v>
       </c>
       <c r="C12" s="3">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D12" s="3">
         <v>5</v>
       </c>
       <c r="E12" s="3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>69</v>
       </c>
       <c r="I12" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J12" s="12">
+        <f t="shared" si="0"/>
+        <v>5.166666666666667</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C13" s="3">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D13" s="3">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E13" s="3">
-        <v>5</v>
+        <v>2</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="H13" s="7" t="s">
+        <v>76</v>
       </c>
       <c r="I13" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J13" s="12">
+        <f t="shared" si="0"/>
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C14" s="3">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D14" s="3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E14" s="3">
-        <v>5</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>37</v>
+        <v>4</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>69</v>
       </c>
       <c r="I14" s="3">
         <v>6</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J14" s="12">
+        <f t="shared" si="0"/>
+        <v>5.333333333333333</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>16</v>
@@ -1064,13 +1199,26 @@
         <v>5</v>
       </c>
       <c r="D15" s="3">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E15" s="3">
-        <v>5</v>
+        <v>1</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>75</v>
       </c>
       <c r="I15" s="3">
         <v>7</v>
+      </c>
+      <c r="J15" s="12">
+        <f t="shared" si="0"/>
+        <v>2.083333333333333</v>
       </c>
     </row>
   </sheetData>
@@ -1081,227 +1229,117 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="4.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="9.140625" style="1"/>
-    <col min="6" max="6" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="57.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="1"/>
+    <col min="3" max="3" width="57.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>21</v>
       </c>
       <c r="B1" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" s="1">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1">
-        <v>0</v>
-      </c>
-      <c r="D2" s="1">
-        <v>2</v>
-      </c>
-      <c r="E2" s="1">
-        <v>0</v>
-      </c>
-      <c r="F2" s="1">
-        <v>1</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B3" s="1">
         <v>2</v>
       </c>
-      <c r="C3" s="1">
-        <v>0</v>
-      </c>
-      <c r="D3" s="1">
-        <v>1</v>
-      </c>
-      <c r="E3" s="1">
-        <v>1</v>
-      </c>
-      <c r="F3" s="1">
-        <v>0</v>
-      </c>
-      <c r="G3" s="1" t="s">
+      <c r="C3" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B4" s="1">
-        <v>1</v>
-      </c>
-      <c r="C4" s="1">
-        <v>3</v>
-      </c>
-      <c r="D4" s="1">
-        <v>0</v>
-      </c>
-      <c r="E4" s="1">
-        <v>0</v>
-      </c>
-      <c r="F4" s="1">
-        <v>1</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="B5" s="1">
         <v>1</v>
       </c>
-      <c r="C5" s="1">
-        <v>3</v>
-      </c>
-      <c r="D5" s="1">
-        <v>0</v>
-      </c>
-      <c r="E5" s="1">
-        <v>0</v>
-      </c>
-      <c r="F5" s="1">
-        <v>0</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C5" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B6" s="1">
-        <v>1</v>
-      </c>
-      <c r="C6" s="1">
-        <v>2</v>
-      </c>
-      <c r="D6" s="1">
-        <v>0</v>
-      </c>
-      <c r="E6" s="1">
-        <v>1</v>
-      </c>
-      <c r="F6" s="1">
-        <v>0</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B7" s="1">
         <v>2</v>
       </c>
-      <c r="C7" s="1">
-        <v>0</v>
-      </c>
-      <c r="D7" s="1">
-        <v>2</v>
-      </c>
-      <c r="E7" s="1">
-        <v>0</v>
-      </c>
-      <c r="F7" s="1">
-        <v>1</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C7" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B8" s="1">
         <v>1</v>
       </c>
-      <c r="C8" s="1">
-        <v>2</v>
-      </c>
-      <c r="D8" s="1">
-        <v>0</v>
-      </c>
-      <c r="E8" s="1">
-        <v>0</v>
-      </c>
-      <c r="F8" s="1">
-        <v>0</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C8" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B9" s="1">
         <v>1</v>
       </c>
-      <c r="C9" s="1">
-        <v>12</v>
-      </c>
-      <c r="D9" s="1">
-        <v>8</v>
-      </c>
-      <c r="E9" s="1">
-        <v>6</v>
-      </c>
-      <c r="F9" s="1">
-        <v>4</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>42</v>
+      <c r="C9" s="1" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -1317,7 +1355,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1327,7 +1365,7 @@
   <sheetData>
     <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B1" s="9" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C1" s="9"/>
       <c r="D1" s="9"/>
@@ -1374,15 +1412,15 @@
       </c>
       <c r="B4" s="1">
         <f>SUM(Cards!C9:C15)</f>
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C4" s="1">
         <f>SUM(Cards!D9:D15)</f>
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="D4" s="1">
         <f>SUM(Cards!E9:E15)</f>
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="E4" s="1">
         <f>SUM(Cards!F9:F15)</f>
@@ -1391,19 +1429,19 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B5" s="1">
         <f>SUM(Cards!C2:C15)</f>
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="C5" s="1">
         <f>SUM(Cards!D2:D15)</f>
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="D5" s="1">
         <f>SUM(Cards!E2:E15)</f>
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="E5" s="1">
         <f>SUM(Cards!F2:F15)</f>

</xml_diff>

<commit_message>
balance and content tweaks for the next playtest
Details:
  * Remove Strange Device and do something that gives you oil (Oil Pan)
  * Better usability on the counter cards - larger squares, etc.
  * Victory conditions written down for once!!
  * Tote bag is more powerful for combat (Have instead of Use)
  *
</commit_message>
<xml_diff>
--- a/game.xlsx
+++ b/game.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Cards" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="82">
   <si>
     <t>Name</t>
   </si>
@@ -118,9 +118,6 @@
     <t>3:1:1 Metal:Fabric:Oil</t>
   </si>
   <si>
-    <t>1:1:1 Metal:Fabric:Oil</t>
-  </si>
-  <si>
     <t>Socket Wrench Puppy</t>
   </si>
   <si>
@@ -130,11 +127,6 @@
     <t>Strong Magnet</t>
   </si>
   <si>
-    <t>1 Oil for 2HP
-or
-2 Fabric for 3 HP</t>
-  </si>
-  <si>
     <t>Bandages</t>
   </si>
   <si>
@@ -153,33 +145,15 @@
     <t>3:1 Metal:Duct Tape</t>
   </si>
   <si>
-    <t>Gain 2 Metal each Round</t>
-  </si>
-  <si>
     <t>Tape Dispensor</t>
   </si>
   <si>
-    <t>Victory!!</t>
-  </si>
-  <si>
-    <t>Zeppelin</t>
-  </si>
-  <si>
-    <t>May convert 3/2/1 Metal/Fabric/Oil to 1 Duct Tape each Round</t>
-  </si>
-  <si>
     <t>Whacking Plank</t>
   </si>
   <si>
     <t>After each battle, may spend 1 Metal for +1 ATK</t>
   </si>
   <si>
-    <t>Strange Device</t>
-  </si>
-  <si>
-    <t>May spend 3 HP for 2 Oil or 2 HP for 1 Fabric any time</t>
-  </si>
-  <si>
     <t>Creature Compositions</t>
   </si>
   <si>
@@ -196,25 +170,12 @@
   </si>
   <si>
     <t>Max</t>
-  </si>
-  <si>
-    <t>7 HP. 2 ATK.</t>
-  </si>
-  <si>
-    <t>1:2 for Metal:Fabric</t>
-  </si>
-  <si>
-    <t>Strong Magnet
-for 4 Metal</t>
   </si>
   <si>
     <t>Tote Bag
 for 3 Fabric</t>
   </si>
   <si>
-    <t>Gain 3 HP after each battle</t>
-  </si>
-  <si>
     <t>1:1 Oil:Duct Tape</t>
   </si>
   <si>
@@ -222,9 +183,6 @@
  ⃠ Use Fireball</t>
   </si>
   <si>
-    <t>Use in battle for -6 Creature HP</t>
-  </si>
-  <si>
     <t>Use for +1 Carry</t>
   </si>
   <si>
@@ -235,10 +193,6 @@
  ⃠ Have Strong Magnet</t>
   </si>
   <si>
-    <t>12 HP. 2 ATK. 
- ⃠ Use Tote Bag</t>
-  </si>
-  <si>
     <t>14 HP. 2 ATK.
  ⃠ Use Bandages</t>
   </si>
@@ -246,10 +200,6 @@
     <t>+1 ATK for 1 Oil</t>
   </si>
   <si>
-    <t>Strong Magnet
-for 3 Metal</t>
-  </si>
-  <si>
     <t>1/2 Tote Bags
 for 2/4 Fabric</t>
   </si>
@@ -281,18 +231,10 @@
 ⃠ Have Whacking Plank</t>
   </si>
   <si>
-    <t>17 HP. 4 ATK. 
-⃠ Have Strange Device</t>
-  </si>
-  <si>
     <t xml:space="preserve">+2 Duct Tape for Disassembling 1 Tool </t>
   </si>
   <si>
     <t>+2 Metal and +2 Fabric for 2 Oil</t>
-  </si>
-  <si>
-    <t>Strange Device
-for 2 Metal, 1 Duct Tape</t>
   </si>
   <si>
     <t>Whacking Plank
@@ -311,12 +253,56 @@
 for 2 Metal, 1 Oil</t>
   </si>
   <si>
-    <t>Strange Device
-for 3 Metal, 1 Duct Tape</t>
-  </si>
-  <si>
     <t>Tape Dispensor
 for 3 Metal, 1 Oil</t>
+  </si>
+  <si>
+    <t>1:1 Metal:Oil
+or
+1:1 Fabric:Oil</t>
+  </si>
+  <si>
+    <t>8 HP. 2 ATK.</t>
+  </si>
+  <si>
+    <t>12 HP. 2 ATK. 
+ ⃠ Have Tote Bag</t>
+  </si>
+  <si>
+    <t>Recover 3/6/9 HP for 1/2/3 Oil</t>
+  </si>
+  <si>
+    <t>Strong Magnet
+for 2 Metal</t>
+  </si>
+  <si>
+    <t>Recover 2 HP for 1 Oil, any time</t>
+  </si>
+  <si>
+    <t>Use in battle for -5 Creature HP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gain 2 Metal at beginning of each Round </t>
+  </si>
+  <si>
+    <t>May convert 3/2/1 Metal/Fabric/Oil to 1 Duct Tape any time</t>
+  </si>
+  <si>
+    <t>Gain +1 Oil after each battle</t>
+  </si>
+  <si>
+    <t>Oil Pan</t>
+  </si>
+  <si>
+    <t>Oil Pan
+for 3 Metal, 1 Duct Tape</t>
+  </si>
+  <si>
+    <t>Oil Pan
+for 2 Metal, 1 Duct Tape</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17 HP. 4 ATK. </t>
   </si>
 </sst>
 </file>
@@ -386,9 +372,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -397,6 +380,9 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -708,8 +694,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -723,7 +709,7 @@
     <col min="7" max="7" width="25.28515625" style="2" customWidth="1"/>
     <col min="8" max="8" width="35.42578125" style="2" customWidth="1"/>
     <col min="9" max="9" width="5" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.140625" style="12"/>
+    <col min="10" max="10" width="9.140625" style="11"/>
     <col min="11" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
@@ -755,8 +741,8 @@
       <c r="I1" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J1" s="11" t="s">
-        <v>70</v>
+      <c r="J1" s="10" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -779,20 +765,20 @@
         <v>25</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>54</v>
+        <v>72</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="I2" s="3">
         <v>1</v>
       </c>
-      <c r="J2" s="12">
+      <c r="J2" s="11">
         <f>C2/4 + D2/3+E2/2</f>
         <v>1.25</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>19</v>
       </c>
@@ -808,26 +794,26 @@
       <c r="E3" s="3">
         <v>3</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>26</v>
+      <c r="F3" s="7" t="s">
+        <v>68</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>82</v>
+        <v>65</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>52</v>
+        <v>69</v>
       </c>
       <c r="I3" s="3">
         <v>2</v>
       </c>
-      <c r="J3" s="12">
+      <c r="J3" s="11">
         <f t="shared" ref="J3:J15" si="0">C3/4 + D3/3+E3/2</f>
         <v>1.8333333333333333</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>8</v>
@@ -842,10 +828,10 @@
         <v>1</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>30</v>
+        <v>71</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>81</v>
+        <v>64</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>10</v>
@@ -853,7 +839,7 @@
       <c r="I4" s="3">
         <v>3</v>
       </c>
-      <c r="J4" s="12">
+      <c r="J4" s="11">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -878,15 +864,15 @@
         <v>12</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>85</v>
+        <v>67</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="I5" s="3">
         <v>4</v>
       </c>
-      <c r="J5" s="12">
+      <c r="J5" s="11">
         <f t="shared" si="0"/>
         <v>1.5833333333333333</v>
       </c>
@@ -908,18 +894,18 @@
         <v>2</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="I6" s="3">
         <v>5</v>
       </c>
-      <c r="J6" s="12">
+      <c r="J6" s="11">
         <f t="shared" si="0"/>
         <v>3.333333333333333</v>
       </c>
@@ -940,19 +926,19 @@
       <c r="E7" s="3">
         <v>0</v>
       </c>
-      <c r="F7" s="10" t="s">
-        <v>65</v>
+      <c r="F7" s="9" t="s">
+        <v>51</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>80</v>
+        <v>63</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="I7" s="3">
         <v>6</v>
       </c>
-      <c r="J7" s="12">
+      <c r="J7" s="11">
         <f t="shared" si="0"/>
         <v>1.9166666666666665</v>
       </c>
@@ -977,15 +963,15 @@
         <v>53</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="I8" s="3">
         <v>7</v>
       </c>
-      <c r="J8" s="12">
+      <c r="J8" s="11">
         <f t="shared" si="0"/>
         <v>2.5833333333333335</v>
       </c>
@@ -1007,18 +993,18 @@
         <v>5</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>83</v>
+        <v>66</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="I9" s="3">
         <v>1</v>
       </c>
-      <c r="J9" s="12">
+      <c r="J9" s="11">
         <f t="shared" si="0"/>
         <v>5.416666666666667</v>
       </c>
@@ -1040,25 +1026,25 @@
         <v>5</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>82</v>
+        <v>65</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="I10" s="3">
         <v>2</v>
       </c>
-      <c r="J10" s="12">
+      <c r="J10" s="11">
         <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>16</v>
@@ -1072,19 +1058,19 @@
       <c r="E11" s="3">
         <v>1</v>
       </c>
-      <c r="F11" s="10" t="s">
-        <v>73</v>
+      <c r="F11" s="9" t="s">
+        <v>58</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="I11" s="3">
         <v>3</v>
       </c>
-      <c r="J11" s="12">
+      <c r="J11" s="11">
         <f t="shared" si="0"/>
         <v>2.5833333333333335</v>
       </c>
@@ -1106,25 +1092,25 @@
         <v>3</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>81</v>
+        <v>64</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="I12" s="3">
         <v>4</v>
       </c>
-      <c r="J12" s="12">
+      <c r="J12" s="11">
         <f t="shared" si="0"/>
         <v>5.166666666666667</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>16</v>
@@ -1139,25 +1125,25 @@
         <v>2</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>68</v>
+        <v>53</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="I13" s="3">
         <v>5</v>
       </c>
-      <c r="J13" s="12">
+      <c r="J13" s="11">
         <f t="shared" si="0"/>
         <v>4.5</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>16</v>
@@ -1171,26 +1157,26 @@
       <c r="E14" s="3">
         <v>4</v>
       </c>
-      <c r="F14" s="10" t="s">
-        <v>77</v>
+      <c r="F14" s="9" t="s">
+        <v>61</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>80</v>
+        <v>63</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="I14" s="3">
         <v>6</v>
       </c>
-      <c r="J14" s="12">
+      <c r="J14" s="11">
         <f t="shared" si="0"/>
         <v>5.333333333333333</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>16</v>
@@ -1204,19 +1190,19 @@
       <c r="E15" s="3">
         <v>1</v>
       </c>
-      <c r="F15" s="10" t="s">
-        <v>78</v>
+      <c r="F15" s="9" t="s">
+        <v>62</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="I15" s="3">
         <v>7</v>
       </c>
-      <c r="J15" s="12">
+      <c r="J15" s="11">
         <f t="shared" si="0"/>
         <v>2.083333333333333</v>
       </c>
@@ -1229,10 +1215,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1248,21 +1234,21 @@
         <v>21</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>56</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -1273,73 +1259,62 @@
         <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>59</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>44</v>
+        <v>78</v>
       </c>
       <c r="B4" s="1">
         <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>45</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B5" s="1">
         <v>1</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>37</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B6" s="1">
         <v>1</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>41</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B7" s="1">
         <v>2</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B8" s="1">
         <v>1</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B9" s="1">
-        <v>1</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1364,12 +1339,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
+      <c r="B1" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
     </row>
     <row r="2" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="4" t="s">
@@ -1429,7 +1404,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="B5" s="1">
         <f>SUM(Cards!C2:C15)</f>

</xml_diff>